<commit_message>
major addition to underwriting process: the connection of the standard mf template to a database which stores rent comp pricing
</commit_message>
<xml_diff>
--- a/app/data/external/States.xlsx
+++ b/app/data/external/States.xlsx
@@ -5,17 +5,17 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\nburmeister\Documents\_Asset Management\_Projects\Asset Management Portal\Database\tables\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\nburmeister\Documents\Development\AssetManagementPortal\app\data\external\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4FE8388C-179A-436F-8C72-DAD100496C83}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D6749AA6-EA8F-416F-9AF9-08C2D62B43DC}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="23625" yWindow="-14205" windowWidth="17280" windowHeight="9210" xr2:uid="{F73C7196-1887-4C80-B5F2-5AF594F13010}"/>
+    <workbookView xWindow="1050" yWindow="-120" windowWidth="27870" windowHeight="16440" xr2:uid="{F73C7196-1887-4C80-B5F2-5AF594F13010}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="191029"/>
+  <calcPr calcId="191029" iterate="1" iterateCount="500"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -550,6 +550,11 @@
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
+  <colors>
+    <mruColors>
+      <color rgb="FF80262A"/>
+    </mruColors>
+  </colors>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
@@ -860,18 +865,18 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EE7F4C58-4C5C-422C-A48B-7504A2AA34F5}">
   <dimension ref="A1:F52"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A37" workbookViewId="0">
-      <selection activeCell="H51" sqref="H51"/>
+    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
+      <selection activeCell="B2" sqref="B2:B52"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="10.33203125" customWidth="1"/>
-    <col min="2" max="2" width="12.21875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="18.6640625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="10.28515625" customWidth="1"/>
+    <col min="2" max="2" width="12.28515625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="18.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -891,7 +896,7 @@
         <v>107</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>1</v>
       </c>
@@ -911,7 +916,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>2</v>
       </c>
@@ -931,7 +936,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>3</v>
       </c>
@@ -951,7 +956,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>4</v>
       </c>
@@ -971,7 +976,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>5</v>
       </c>
@@ -991,7 +996,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>6</v>
       </c>
@@ -1011,7 +1016,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>7</v>
       </c>
@@ -1031,7 +1036,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A9">
         <v>8</v>
       </c>
@@ -1051,7 +1056,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A10">
         <v>9</v>
       </c>
@@ -1071,7 +1076,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A11">
         <v>10</v>
       </c>
@@ -1091,7 +1096,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A12">
         <v>11</v>
       </c>
@@ -1111,7 +1116,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A13">
         <v>12</v>
       </c>
@@ -1131,7 +1136,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A14">
         <v>13</v>
       </c>
@@ -1151,7 +1156,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A15">
         <v>14</v>
       </c>
@@ -1171,7 +1176,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A16">
         <v>15</v>
       </c>
@@ -1191,7 +1196,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A17">
         <v>16</v>
       </c>
@@ -1211,7 +1216,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A18">
         <v>17</v>
       </c>
@@ -1231,7 +1236,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A19">
         <v>18</v>
       </c>
@@ -1251,7 +1256,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A20">
         <v>19</v>
       </c>
@@ -1271,7 +1276,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="21" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A21">
         <v>20</v>
       </c>
@@ -1291,7 +1296,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="22" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A22">
         <v>21</v>
       </c>
@@ -1311,7 +1316,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="23" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A23">
         <v>22</v>
       </c>
@@ -1331,7 +1336,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="24" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A24">
         <v>23</v>
       </c>
@@ -1351,7 +1356,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="25" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A25">
         <v>24</v>
       </c>
@@ -1371,7 +1376,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="26" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A26">
         <v>25</v>
       </c>
@@ -1391,7 +1396,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="27" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A27">
         <v>26</v>
       </c>
@@ -1411,7 +1416,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="28" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A28">
         <v>27</v>
       </c>
@@ -1431,7 +1436,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="29" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A29">
         <v>28</v>
       </c>
@@ -1451,7 +1456,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="30" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A30">
         <v>29</v>
       </c>
@@ -1471,7 +1476,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="31" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A31">
         <v>30</v>
       </c>
@@ -1491,7 +1496,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="32" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A32">
         <v>31</v>
       </c>
@@ -1511,7 +1516,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="33" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A33">
         <v>32</v>
       </c>
@@ -1531,7 +1536,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="34" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A34">
         <v>33</v>
       </c>
@@ -1551,7 +1556,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="35" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A35">
         <v>34</v>
       </c>
@@ -1571,7 +1576,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="36" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A36">
         <v>35</v>
       </c>
@@ -1591,7 +1596,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="37" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A37">
         <v>36</v>
       </c>
@@ -1611,7 +1616,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="38" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A38">
         <v>37</v>
       </c>
@@ -1631,7 +1636,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="39" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A39">
         <v>38</v>
       </c>
@@ -1651,7 +1656,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="40" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A40">
         <v>39</v>
       </c>
@@ -1671,7 +1676,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="41" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A41">
         <v>40</v>
       </c>
@@ -1691,7 +1696,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="42" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A42">
         <v>41</v>
       </c>
@@ -1711,7 +1716,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="43" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A43">
         <v>42</v>
       </c>
@@ -1731,7 +1736,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="44" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A44">
         <v>43</v>
       </c>
@@ -1751,7 +1756,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="45" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A45">
         <v>44</v>
       </c>
@@ -1771,7 +1776,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="46" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A46">
         <v>45</v>
       </c>
@@ -1791,7 +1796,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="47" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A47">
         <v>46</v>
       </c>
@@ -1811,7 +1816,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="48" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="48" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A48">
         <v>47</v>
       </c>
@@ -1831,7 +1836,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="49" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="49" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A49">
         <v>48</v>
       </c>
@@ -1851,7 +1856,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="50" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="50" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A50">
         <v>49</v>
       </c>
@@ -1871,7 +1876,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="51" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="51" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A51">
         <v>50</v>
       </c>
@@ -1891,7 +1896,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="52" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="52" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A52">
         <v>51</v>
       </c>

</xml_diff>